<commit_message>
merge additional data into original dataset
</commit_message>
<xml_diff>
--- a/02 exclusion results based on paper contents.xlsx
+++ b/02 exclusion results based on paper contents.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Paper\MDE4DTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CFC4FEA4-661F-44DE-B3DE-BEFEDD4963BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D21AC931-9FF4-4ECF-9BC1-AD0F9D135B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2490" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="extraction_merged" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">extraction_merged!$A$1:$G$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">extraction_merged!$A$1:$F$78</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="293" uniqueCount="88">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="381" uniqueCount="112">
   <si>
     <t>Title</t>
   </si>
@@ -292,9 +292,6 @@
     <t>Integration of SysML Models in a 3D Environment for Virtual Testing and Validation</t>
   </si>
   <si>
-    <t>klassische Model Comparison</t>
-  </si>
-  <si>
     <t>Decision</t>
   </si>
   <si>
@@ -302,13 +299,88 @@
   </si>
   <si>
     <t>No MDE application</t>
+  </si>
+  <si>
+    <t>A data- and model-driven approach for cancer treatment</t>
+  </si>
+  <si>
+    <t>A digital twin-driven hybrid approach for the prediction of performance degradation in transmission unit of CNC machine tool</t>
+  </si>
+  <si>
+    <t>A multi-model ensemble digital twin solution for real-time unsteady flow state estimation of a pumping station</t>
+  </si>
+  <si>
+    <t>A virtual model knowledge updating method driven by data</t>
+  </si>
+  <si>
+    <t>An EV-Traction Inverter Data-Driven Modelling for Digital Twin Development</t>
+  </si>
+  <si>
+    <t>Classification and Mapping of Layout Algorithms for Usage in Graph-like Modeling Languages</t>
+  </si>
+  <si>
+    <t>Concept of a Modular and System Model Driven Digital Twin for Engineering Education</t>
+  </si>
+  <si>
+    <t>Data-Driven Methodology to Support Long-Lasting Logistics and Decision Making for Urban Last-Mile Operations</t>
+  </si>
+  <si>
+    <t>Decentralized Autonomous Operations and Organizations in TransVerse: Federated Intelligence for Smart Mobility</t>
+  </si>
+  <si>
+    <t>Digital Behavioral Twins for Safe Connected Cars</t>
+  </si>
+  <si>
+    <t>Digital modeling-driven chatter suppression for thin-walled part manufacturing</t>
+  </si>
+  <si>
+    <t>Digital Twin Driven Green Performance Evaluation Methodology of Intelligent Manufacturing: Hybrid Model Based on Fuzzy Rough-Sets AHP, Multistage Weight Synthesis, and PROMETHEE II</t>
+  </si>
+  <si>
+    <t>Digital Twins for Sustainable Software Systems</t>
+  </si>
+  <si>
+    <t>Dynamic Runtime Integration of New Models in Digital Twins</t>
+  </si>
+  <si>
+    <t>EMF-Syncer: scalable maintenance of view models over heterogeneous data-centric software systems at run time</t>
+  </si>
+  <si>
+    <t>GRuM-A flexible model-driven runtime monitoring framework and its application to automated aerial and ground vehicles</t>
+  </si>
+  <si>
+    <t>On the Notion of Digital Twins: A Modeling Perspective</t>
+  </si>
+  <si>
+    <t>Reliable Counterparts: Efficiently Testing Causal Relationships in Digital Twins</t>
+  </si>
+  <si>
+    <t>Simulation-Based Engineering of Heterogeneous Collaborative Systems-A Novel Conceptual Framework</t>
+  </si>
+  <si>
+    <t>Supporting Digital Twins for the Retrofit in Aviation by a Model-Driven Data Handling</t>
+  </si>
+  <si>
+    <t>Supporting the Implementation of Digital Twins for IoT-Enhanced BPs</t>
+  </si>
+  <si>
+    <t>TwinOps - DevOps Meets Model-Based Engineering and Digital Twins for the Engineering of CPS</t>
+  </si>
+  <si>
+    <t>UAV-Assisted Three-Dimensional Spectrum Mapping Driven by Spectrum Data and Channel Model</t>
+  </si>
+  <si>
+    <t>No DT used</t>
+  </si>
+  <si>
+    <t>To be discuessed with Manuel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -452,6 +524,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -804,12 +883,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1165,25 +1245,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A65" sqref="A65"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="141.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="141.1015625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.88671875" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="21.89453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.68359375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1199,11 +1278,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1219,48 +1298,48 @@
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4" t="str">
+      <c r="F2" s="4" t="str">
         <f>E2</f>
         <v>OK</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" s="4" t="str">
-        <f t="shared" ref="G3:G64" si="0">E3</f>
+        <v>85</v>
+      </c>
+      <c r="F3" s="4" t="str">
+        <f t="shared" ref="F3:F62" si="0">E3</f>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G4" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F4" s="4" t="str">
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1273,15 +1352,12 @@
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="4" t="str">
+      <c r="F5" s="4" t="str">
         <f>E5</f>
         <v>No Model used</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1289,35 +1365,35 @@
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="4" t="str">
+      <c r="F6" s="4" t="str">
         <f>E6</f>
         <v>OK</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G7" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1330,35 +1406,35 @@
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="4" t="str">
+      <c r="F8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>6</v>
@@ -1366,30 +1442,30 @@
       <c r="E10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="4" t="str">
+      <c r="F10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G11" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1402,12 +1478,12 @@
       <c r="E12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="4" t="str">
+      <c r="F12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1415,22 +1491,22 @@
         <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G13" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F13" s="4" t="str">
         <f>E13</f>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>6</v>
@@ -1438,12 +1514,12 @@
       <c r="E14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="4" t="str">
+      <c r="F14" s="4" t="str">
         <f>E14</f>
         <v>OK</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1456,45 +1532,45 @@
       <c r="E15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="4" t="str">
+      <c r="F15" s="4" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G16" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F16" s="4" t="str">
         <f>E16</f>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G17" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F17" s="4" t="str">
         <f>D17</f>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1507,27 +1583,27 @@
       <c r="D18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="4" t="str">
-        <f t="shared" ref="G18:G28" si="1">D18</f>
+      <c r="F18" s="4" t="str">
+        <f t="shared" ref="F18:F28" si="1">D18</f>
         <v>OK</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F19" s="4" t="str">
         <f t="shared" si="1"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -1540,72 +1616,72 @@
       <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="4" t="str">
+      <c r="F20" s="4" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G21" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F21" s="4" t="str">
         <f t="shared" si="1"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G22" s="4" t="str">
+        <v>85</v>
+      </c>
+      <c r="F22" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G23" s="4" t="str">
+        <v>85</v>
+      </c>
+      <c r="F23" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G24" s="4" t="str">
+        <v>85</v>
+      </c>
+      <c r="F24" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -1618,45 +1694,45 @@
       <c r="D25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="4" t="str">
+      <c r="F25" s="4" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G26" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F26" s="4" t="str">
         <f t="shared" si="1"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G27" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F27" s="4" t="str">
         <f t="shared" si="1"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1669,12 +1745,12 @@
       <c r="D28" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G28" s="4" t="str">
+      <c r="F28" s="4" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
@@ -1687,12 +1763,12 @@
       <c r="D29" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="4" t="str">
+      <c r="F29" s="4" t="str">
         <f>D29</f>
         <v>No Model used</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
@@ -1700,17 +1776,17 @@
         <v>10</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G30" s="4" t="str">
+      <c r="F30" s="4" t="str">
         <f>D30</f>
         <v>No Model used</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
@@ -1718,65 +1794,65 @@
         <v>10</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G31" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F31" s="4" t="str">
         <f>D31</f>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G32" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F32" s="4" t="str">
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G33" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F33" s="4" t="str">
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G34" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F34" s="4" t="str">
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2" t="s">
         <v>40</v>
       </c>
@@ -1789,12 +1865,12 @@
       <c r="E35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G35" s="4" t="str">
+      <c r="F35" s="4" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
@@ -1807,12 +1883,12 @@
       <c r="E36" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G36" s="4" t="str">
+      <c r="F36" s="4" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2" t="s">
         <v>42</v>
       </c>
@@ -1823,13 +1899,13 @@
         <v>6</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
@@ -1842,92 +1918,92 @@
       <c r="E38" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="4" t="str">
+      <c r="F38" s="4" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G39" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F39" s="4" t="str">
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G40" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F40" s="4" t="str">
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G41" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F41" s="4" t="str">
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G42" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F42" s="4" t="str">
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G43" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F43" s="4" t="str">
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>6</v>
@@ -1935,38 +2011,38 @@
       <c r="E44" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G44" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F44" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G45" s="4"/>
-    </row>
-    <row r="46" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G46" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F46" s="4" t="str">
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2" t="s">
         <v>52</v>
       </c>
@@ -1974,14 +2050,14 @@
         <v>10</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G47" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F47" s="4" t="str">
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
@@ -1994,12 +2070,12 @@
       <c r="E48" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="4" t="str">
+      <c r="F48" s="4" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2" t="s">
         <v>54</v>
       </c>
@@ -2012,12 +2088,12 @@
       <c r="E49" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G49" s="4" t="str">
+      <c r="F49" s="4" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="2" t="s">
         <v>55</v>
       </c>
@@ -2030,12 +2106,12 @@
       <c r="E50" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G50" s="4" t="str">
+      <c r="F50" s="4" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2" t="s">
         <v>56</v>
       </c>
@@ -2048,12 +2124,12 @@
       <c r="E51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G51" s="4" t="str">
+      <c r="F51" s="4" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="2" t="s">
         <v>57</v>
       </c>
@@ -2066,110 +2142,110 @@
       <c r="E52" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G52" s="4" t="str">
+      <c r="F52" s="4" t="str">
         <f t="shared" si="0"/>
         <v>No Model used</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G53" s="4" t="str">
+        <v>85</v>
+      </c>
+      <c r="F53" s="4" t="str">
         <f>D53</f>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G54" s="4" t="str">
-        <f t="shared" ref="G54:G57" si="2">D54</f>
-        <v>No MDE application</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="F54" s="4" t="str">
+        <f t="shared" ref="F54:F56" si="2">D54</f>
+        <v>No MDE application</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G55" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F55" s="4" t="str">
         <f t="shared" si="2"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G56" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F56" s="4" t="str">
         <f t="shared" si="2"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G58" s="4" t="str">
+        <v>85</v>
+      </c>
+      <c r="F58" s="4" t="str">
         <f>E58</f>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="59" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2" t="s">
         <v>64</v>
       </c>
@@ -2177,17 +2253,17 @@
         <v>6</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G59" s="4" t="str">
+        <v>85</v>
+      </c>
+      <c r="F59" s="4" t="str">
         <f>E59</f>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="2" t="s">
         <v>65</v>
       </c>
@@ -2200,12 +2276,12 @@
       <c r="E60" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G60" s="4" t="str">
+      <c r="F60" s="4" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="2" t="s">
         <v>66</v>
       </c>
@@ -2218,30 +2294,30 @@
       <c r="E61" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G61" s="4" t="str">
+      <c r="F61" s="4" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G62" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F62" s="4" t="str">
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="2" t="s">
         <v>68</v>
       </c>
@@ -2254,30 +2330,30 @@
       <c r="D63" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G63" s="4" t="str">
-        <f t="shared" ref="G63:G70" si="3">D63</f>
+      <c r="F63" s="4" t="str">
+        <f t="shared" ref="F63:F70" si="3">D63</f>
         <v>OK</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G64" s="4" t="str">
+      <c r="F64" s="4" t="str">
         <f>C64</f>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="2" t="s">
         <v>70</v>
       </c>
@@ -2290,72 +2366,72 @@
       <c r="E65" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G65" s="4" t="str">
+      <c r="F65" s="4" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G66" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F66" s="4" t="str">
         <f t="shared" si="3"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G67" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F67" s="4" t="str">
         <f t="shared" si="3"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G68" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F68" s="4" t="str">
         <f t="shared" si="3"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G69" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F69" s="4" t="str">
         <f t="shared" si="3"/>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="2" t="s">
         <v>75</v>
       </c>
@@ -2368,12 +2444,12 @@
       <c r="E70" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G70" s="4" t="str">
+      <c r="F70" s="4" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="2" t="s">
         <v>76</v>
       </c>
@@ -2386,26 +2462,26 @@
       <c r="E71" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G71" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F71" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G72" s="4" t="str">
+        <v>86</v>
+      </c>
+      <c r="F72" s="4" t="str">
         <f>D72</f>
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="2" t="s">
         <v>78</v>
       </c>
@@ -2418,12 +2494,12 @@
       <c r="D73" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G73" s="4" t="str">
+      <c r="F73" s="4" t="str">
         <f>D73</f>
         <v>OK</v>
       </c>
     </row>
-    <row r="74" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="2" t="s">
         <v>79</v>
       </c>
@@ -2436,42 +2512,42 @@
       <c r="E74" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G74" s="4" t="str">
-        <f t="shared" ref="G74:G78" si="4">E74</f>
+      <c r="F74" s="4" t="str">
+        <f t="shared" ref="F74:F78" si="4">E74</f>
         <v>OK</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="2" t="s">
         <v>80</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G75" s="4" t="str">
+        <v>85</v>
+      </c>
+      <c r="F75" s="4" t="str">
         <f t="shared" si="4"/>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="76" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G76" s="4" t="str">
+        <v>85</v>
+      </c>
+      <c r="F76" s="4" t="str">
         <f t="shared" si="4"/>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="2" t="s">
         <v>82</v>
       </c>
@@ -2484,12 +2560,12 @@
       <c r="E77" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G77" s="4" t="str">
+      <c r="F77" s="4" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="2" t="s">
         <v>83</v>
       </c>
@@ -2502,20 +2578,350 @@
       <c r="E78" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G78" s="4" t="str">
+      <c r="F78" s="4" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" t="s">
+        <v>87</v>
+      </c>
       <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
+      <c r="C79" t="s">
+        <v>86</v>
+      </c>
+      <c r="D79" t="s">
+        <v>86</v>
+      </c>
+      <c r="E79" t="s">
+        <v>85</v>
+      </c>
+      <c r="F79" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" t="s">
+        <v>88</v>
+      </c>
+      <c r="C80" s="5"/>
+      <c r="D80" t="s">
+        <v>86</v>
+      </c>
+      <c r="E80" t="s">
+        <v>86</v>
+      </c>
+      <c r="F80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" t="s">
+        <v>89</v>
+      </c>
+      <c r="C81" t="s">
+        <v>86</v>
+      </c>
+      <c r="D81" t="s">
+        <v>86</v>
+      </c>
+      <c r="E81" t="s">
+        <v>86</v>
+      </c>
+      <c r="F81" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" t="s">
+        <v>90</v>
+      </c>
+      <c r="D82" t="s">
+        <v>86</v>
+      </c>
+      <c r="E82" t="s">
+        <v>86</v>
+      </c>
+      <c r="F82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" t="s">
+        <v>91</v>
+      </c>
+      <c r="C83" t="s">
+        <v>86</v>
+      </c>
+      <c r="D83" t="s">
+        <v>86</v>
+      </c>
+      <c r="F83" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" t="s">
+        <v>92</v>
+      </c>
+      <c r="C84" t="s">
+        <v>86</v>
+      </c>
+      <c r="D84" t="s">
+        <v>110</v>
+      </c>
+      <c r="E84" t="s">
+        <v>110</v>
+      </c>
+      <c r="F84" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" t="s">
+        <v>94</v>
+      </c>
+      <c r="C86" t="s">
+        <v>86</v>
+      </c>
+      <c r="D86" t="s">
+        <v>86</v>
+      </c>
+      <c r="E86" t="s">
+        <v>86</v>
+      </c>
+      <c r="F86" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" t="s">
+        <v>95</v>
+      </c>
+      <c r="C87" t="s">
+        <v>86</v>
+      </c>
+      <c r="D87" t="s">
+        <v>86</v>
+      </c>
+      <c r="E87" t="s">
+        <v>86</v>
+      </c>
+      <c r="F87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" t="s">
+        <v>96</v>
+      </c>
+      <c r="C88" t="s">
+        <v>86</v>
+      </c>
+      <c r="D88" t="s">
+        <v>86</v>
+      </c>
+      <c r="E88" t="s">
+        <v>86</v>
+      </c>
+      <c r="F88" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" t="s">
+        <v>97</v>
+      </c>
+      <c r="C89" t="s">
+        <v>86</v>
+      </c>
+      <c r="D89" t="s">
+        <v>86</v>
+      </c>
+      <c r="E89" t="s">
+        <v>86</v>
+      </c>
+      <c r="F89" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" t="s">
+        <v>98</v>
+      </c>
+      <c r="C90" t="s">
+        <v>86</v>
+      </c>
+      <c r="D90" t="s">
+        <v>86</v>
+      </c>
+      <c r="F90" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" t="s">
+        <v>99</v>
+      </c>
+      <c r="C91" t="s">
+        <v>85</v>
+      </c>
+      <c r="D91" t="s">
+        <v>85</v>
+      </c>
+      <c r="E91" t="s">
+        <v>85</v>
+      </c>
+      <c r="F91" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" t="s">
+        <v>100</v>
+      </c>
+      <c r="C92" t="s">
+        <v>86</v>
+      </c>
+      <c r="E92" t="s">
+        <v>86</v>
+      </c>
+      <c r="F92" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" t="s">
+        <v>101</v>
+      </c>
+      <c r="C93" t="s">
+        <v>110</v>
+      </c>
+      <c r="D93" s="5"/>
+      <c r="E93" t="s">
+        <v>110</v>
+      </c>
+      <c r="F93" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" t="s">
+        <v>102</v>
+      </c>
+      <c r="C94" t="s">
+        <v>110</v>
+      </c>
+      <c r="D94" t="s">
+        <v>110</v>
+      </c>
+      <c r="E94" t="s">
+        <v>110</v>
+      </c>
+      <c r="F94" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" t="s">
+        <v>103</v>
+      </c>
+      <c r="C95" t="s">
+        <v>85</v>
+      </c>
+      <c r="D95" t="s">
+        <v>86</v>
+      </c>
+      <c r="F95" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" t="s">
+        <v>105</v>
+      </c>
+      <c r="C97" t="s">
+        <v>86</v>
+      </c>
+      <c r="D97" t="s">
+        <v>86</v>
+      </c>
+      <c r="F97" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" t="s">
+        <v>109</v>
+      </c>
+      <c r="C101" t="s">
+        <v>86</v>
+      </c>
+      <c r="D101" t="s">
+        <v>86</v>
+      </c>
+      <c r="E101" t="s">
+        <v>86</v>
+      </c>
+      <c r="F101" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F102"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G78" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F78" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2527,7 +2933,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update figure names + add template for 3d figure
</commit_message>
<xml_diff>
--- a/02 exclusion results based on paper contents.xlsx
+++ b/02 exclusion results based on paper contents.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Paper\MDE4DTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D21AC931-9FF4-4ECF-9BC1-AD0F9D135B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8C74D2C5-36D6-4C8B-A752-6C5D0FDC44B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="2490" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="extraction_merged" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">extraction_merged!$A$1:$F$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">extraction_merged!$A$1:$F$101</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="381" uniqueCount="112">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="386" uniqueCount="112">
   <si>
     <t>Title</t>
   </si>
@@ -1247,22 +1247,22 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="141.1015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="141.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="21.89453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>No Model used</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>No Model used</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>No Model used</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>40</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>42</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>45</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>46</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>50</v>
       </c>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>52</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>54</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>55</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>56</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>57</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>No Model used</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>58</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>60</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>61</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>62</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>63</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>64</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>65</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>66</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>67</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>68</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>69</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>70</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>71</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>72</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>73</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>74</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>75</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>76</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>77</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>No MDE application</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>78</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>79</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>80</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>81</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>82</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="78" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>83</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>87</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>88</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>89</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>90</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>92</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>93</v>
       </c>
@@ -2687,9 +2687,11 @@
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
-      <c r="F85" s="5"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F85" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>94</v>
       </c>
@@ -2706,7 +2708,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>95</v>
       </c>
@@ -2723,7 +2725,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>96</v>
       </c>
@@ -2740,7 +2742,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>97</v>
       </c>
@@ -2757,7 +2759,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>98</v>
       </c>
@@ -2771,7 +2773,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>99</v>
       </c>
@@ -2788,7 +2790,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>100</v>
       </c>
@@ -2802,7 +2804,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>101</v>
       </c>
@@ -2817,7 +2819,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>102</v>
       </c>
@@ -2834,7 +2836,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>103</v>
       </c>
@@ -2848,16 +2850,18 @@
         <v>86</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>104</v>
       </c>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
       <c r="E96" s="5"/>
-      <c r="F96" s="5"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F96" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>105</v>
       </c>
@@ -2871,7 +2875,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>106</v>
       </c>
@@ -2880,27 +2884,33 @@
       </c>
       <c r="D98" s="5"/>
       <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F98" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>107</v>
       </c>
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
       <c r="E99" s="5"/>
-      <c r="F99" s="5"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F99" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>108</v>
       </c>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
       <c r="E100" s="5"/>
-      <c r="F100" s="5"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F100" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>109</v>
       </c>
@@ -2917,11 +2927,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F102"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F78" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F101" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2933,7 +2943,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cleanup + describe reviewing of exclusion decisions
</commit_message>
<xml_diff>
--- a/02 exclusion results based on paper contents.xlsx
+++ b/02 exclusion results based on paper contents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Paper\MDE4DTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8C74D2C5-36D6-4C8B-A752-6C5D0FDC44B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6DB1A429-86C7-4F18-AB95-0EA16ECE3FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2490" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="extraction_merged" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="386" uniqueCount="112">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="430" uniqueCount="114">
   <si>
     <t>Title</t>
   </si>
@@ -373,14 +373,20 @@
     <t>No DT used</t>
   </si>
   <si>
-    <t>To be discuessed with Manuel</t>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Veto?</t>
+  </si>
+  <si>
+    <t>Decision after Veto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -528,15 +534,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -714,12 +713,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -883,13 +876,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1245,24 +1239,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomLeft" activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="141.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="141.15625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="21.83984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.41796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1281,8 +1276,14 @@
       <c r="F1" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1302,8 +1303,10 @@
         <f>E2</f>
         <v>OK</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1320,8 +1323,10 @@
         <f t="shared" ref="F3:F62" si="0">E3</f>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1334,12 +1339,17 @@
       <c r="E4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>No MDE application</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1352,12 +1362,17 @@
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="4" t="str">
-        <f>E5</f>
-        <v>No Model used</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1374,8 +1389,10 @@
         <f>E6</f>
         <v>OK</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1392,8 +1409,10 @@
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1410,8 +1429,10 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1428,8 +1449,10 @@
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1446,8 +1469,10 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1464,8 +1489,10 @@
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1482,8 +1509,10 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1500,8 +1529,10 @@
         <f>E13</f>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1518,8 +1549,10 @@
         <f>E14</f>
         <v>OK</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1536,8 +1569,10 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -1550,12 +1585,17 @@
       <c r="E16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="4" t="str">
-        <f>E16</f>
-        <v>No MDE application</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1565,12 +1605,17 @@
       <c r="D17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F17" s="4" t="str">
-        <f>D17</f>
-        <v>No MDE application</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1587,8 +1632,10 @@
         <f t="shared" ref="F18:F28" si="1">D18</f>
         <v>OK</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1602,8 +1649,10 @@
         <f t="shared" si="1"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -1620,8 +1669,10 @@
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
@@ -1631,12 +1682,17 @@
       <c r="D21" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F21" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>No MDE application</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
@@ -1650,8 +1706,10 @@
         <f t="shared" si="1"/>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
@@ -1665,8 +1723,10 @@
         <f t="shared" si="1"/>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
@@ -1680,8 +1740,10 @@
         <f t="shared" si="1"/>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -1698,8 +1760,10 @@
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
@@ -1713,8 +1777,10 @@
         <f t="shared" si="1"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -1731,8 +1797,10 @@
         <f t="shared" si="1"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1749,8 +1817,10 @@
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
@@ -1767,8 +1837,10 @@
         <f>D29</f>
         <v>No Model used</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
@@ -1785,8 +1857,10 @@
         <f>D30</f>
         <v>No Model used</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
@@ -1803,8 +1877,10 @@
         <f>D31</f>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
@@ -1821,8 +1897,10 @@
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
@@ -1836,8 +1914,10 @@
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -1851,8 +1931,10 @@
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2" t="s">
         <v>40</v>
       </c>
@@ -1869,8 +1951,10 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
@@ -1887,8 +1971,10 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2" t="s">
         <v>42</v>
       </c>
@@ -1904,8 +1990,10 @@
       <c r="F37" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
@@ -1922,8 +2010,10 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
@@ -1937,8 +2027,10 @@
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2" t="s">
         <v>45</v>
       </c>
@@ -1948,12 +2040,13 @@
       <c r="E40" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>No MDE application</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2" t="s">
         <v>46</v>
       </c>
@@ -1967,8 +2060,10 @@
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
@@ -1982,8 +2077,10 @@
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
@@ -1997,8 +2094,10 @@
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
@@ -2014,8 +2113,10 @@
       <c r="F44" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2" t="s">
         <v>50</v>
       </c>
@@ -2026,8 +2127,10 @@
         <v>85</v>
       </c>
       <c r="F45" s="4"/>
-    </row>
-    <row r="46" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -2041,8 +2144,10 @@
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2" t="s">
         <v>52</v>
       </c>
@@ -2056,8 +2161,10 @@
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
@@ -2074,8 +2181,10 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2" t="s">
         <v>54</v>
       </c>
@@ -2092,8 +2201,10 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="2" t="s">
         <v>55</v>
       </c>
@@ -2110,8 +2221,10 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2" t="s">
         <v>56</v>
       </c>
@@ -2128,8 +2241,10 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="2" t="s">
         <v>57</v>
       </c>
@@ -2146,8 +2261,10 @@
         <f t="shared" si="0"/>
         <v>No Model used</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="2" t="s">
         <v>58</v>
       </c>
@@ -2161,8 +2278,10 @@
         <f>D53</f>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
@@ -2175,12 +2294,17 @@
       <c r="E54" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F54" s="4" t="str">
-        <f t="shared" ref="F54:F56" si="2">D54</f>
-        <v>No MDE application</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F54" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="2" t="s">
         <v>60</v>
       </c>
@@ -2190,12 +2314,17 @@
       <c r="D55" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F55" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>No MDE application</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F55" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="2" t="s">
         <v>61</v>
       </c>
@@ -2208,12 +2337,17 @@
       <c r="D56" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F56" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>No MDE application</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="2" t="s">
         <v>62</v>
       </c>
@@ -2226,8 +2360,10 @@
       <c r="F57" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+    </row>
+    <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2" t="s">
         <v>63</v>
       </c>
@@ -2244,8 +2380,10 @@
         <f>E58</f>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+    </row>
+    <row r="59" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2" t="s">
         <v>64</v>
       </c>
@@ -2262,8 +2400,10 @@
         <f>E59</f>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+    </row>
+    <row r="60" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="2" t="s">
         <v>65</v>
       </c>
@@ -2280,8 +2420,10 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+    </row>
+    <row r="61" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="2" t="s">
         <v>66</v>
       </c>
@@ -2298,8 +2440,10 @@
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+    </row>
+    <row r="62" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="2" t="s">
         <v>67</v>
       </c>
@@ -2316,8 +2460,10 @@
         <f t="shared" si="0"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+    </row>
+    <row r="63" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="2" t="s">
         <v>68</v>
       </c>
@@ -2331,11 +2477,13 @@
         <v>6</v>
       </c>
       <c r="F63" s="4" t="str">
-        <f t="shared" ref="F63:F70" si="3">D63</f>
+        <f t="shared" ref="F63:F70" si="2">D63</f>
         <v>OK</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+    </row>
+    <row r="64" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="2" t="s">
         <v>69</v>
       </c>
@@ -2352,8 +2500,10 @@
         <f>C64</f>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+    </row>
+    <row r="65" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="2" t="s">
         <v>70</v>
       </c>
@@ -2367,11 +2517,13 @@
         <v>6</v>
       </c>
       <c r="F65" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+    </row>
+    <row r="66" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="2" t="s">
         <v>71</v>
       </c>
@@ -2381,12 +2533,17 @@
       <c r="D66" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F66" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>No MDE application</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F66" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="2" t="s">
         <v>72</v>
       </c>
@@ -2397,11 +2554,13 @@
         <v>86</v>
       </c>
       <c r="F67" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+    </row>
+    <row r="68" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="2" t="s">
         <v>73</v>
       </c>
@@ -2412,11 +2571,13 @@
         <v>86</v>
       </c>
       <c r="F68" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>No MDE application</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+    </row>
+    <row r="69" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="2" t="s">
         <v>74</v>
       </c>
@@ -2426,12 +2587,17 @@
       <c r="D69" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F69" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>No MDE application</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F69" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="2" t="s">
         <v>75</v>
       </c>
@@ -2445,11 +2611,13 @@
         <v>6</v>
       </c>
       <c r="F70" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+    </row>
+    <row r="71" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="2" t="s">
         <v>76</v>
       </c>
@@ -2465,8 +2633,10 @@
       <c r="F71" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+    </row>
+    <row r="72" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="2" t="s">
         <v>77</v>
       </c>
@@ -2476,12 +2646,17 @@
       <c r="D72" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F72" s="4" t="str">
-        <f>D72</f>
-        <v>No MDE application</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F72" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="2" t="s">
         <v>78</v>
       </c>
@@ -2498,8 +2673,10 @@
         <f>D73</f>
         <v>OK</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+    </row>
+    <row r="74" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="2" t="s">
         <v>79</v>
       </c>
@@ -2513,11 +2690,13 @@
         <v>6</v>
       </c>
       <c r="F74" s="4" t="str">
-        <f t="shared" ref="F74:F78" si="4">E74</f>
+        <f t="shared" ref="F74:F78" si="3">E74</f>
         <v>OK</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+    </row>
+    <row r="75" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="2" t="s">
         <v>80</v>
       </c>
@@ -2528,11 +2707,13 @@
         <v>85</v>
       </c>
       <c r="F75" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+    </row>
+    <row r="76" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="2" t="s">
         <v>81</v>
       </c>
@@ -2543,11 +2724,13 @@
         <v>85</v>
       </c>
       <c r="F76" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>Philosophical, Opinion, or Experience paper</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+    </row>
+    <row r="77" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="2" t="s">
         <v>82</v>
       </c>
@@ -2561,11 +2744,13 @@
         <v>6</v>
       </c>
       <c r="F77" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+    </row>
+    <row r="78" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="2" t="s">
         <v>83</v>
       </c>
@@ -2579,356 +2764,409 @@
         <v>6</v>
       </c>
       <c r="F78" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B79" s="2"/>
-      <c r="C79" t="s">
-        <v>86</v>
-      </c>
-      <c r="D79" t="s">
-        <v>86</v>
-      </c>
-      <c r="E79" t="s">
+      <c r="C79" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E79" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F79" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+      <c r="F79" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C80" s="5"/>
-      <c r="D80" t="s">
-        <v>86</v>
-      </c>
-      <c r="E80" t="s">
-        <v>86</v>
-      </c>
-      <c r="F80" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C81" t="s">
-        <v>86</v>
-      </c>
-      <c r="D81" t="s">
-        <v>86</v>
-      </c>
-      <c r="E81" t="s">
-        <v>86</v>
-      </c>
-      <c r="F81" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+      <c r="B81" s="2"/>
+      <c r="C81" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D82" t="s">
-        <v>86</v>
-      </c>
-      <c r="E82" t="s">
-        <v>86</v>
-      </c>
-      <c r="F82" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C83" t="s">
-        <v>86</v>
-      </c>
-      <c r="D83" t="s">
-        <v>86</v>
-      </c>
-      <c r="F83" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+      <c r="B83" s="2"/>
+      <c r="C83" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E83" s="2"/>
+      <c r="F83" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C84" t="s">
-        <v>86</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="B84" s="2"/>
+      <c r="C84" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F84" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="5" t="s">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C85" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5"/>
-      <c r="F85" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+      <c r="B85" s="2"/>
+      <c r="C85" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C86" t="s">
-        <v>86</v>
-      </c>
-      <c r="D86" t="s">
-        <v>86</v>
-      </c>
-      <c r="E86" t="s">
-        <v>86</v>
-      </c>
-      <c r="F86" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+      <c r="B86" s="2"/>
+      <c r="C86" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C87" t="s">
-        <v>86</v>
-      </c>
-      <c r="D87" t="s">
-        <v>86</v>
-      </c>
-      <c r="E87" t="s">
-        <v>86</v>
-      </c>
-      <c r="F87" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+      <c r="B87" s="2"/>
+      <c r="C87" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C88" t="s">
-        <v>86</v>
-      </c>
-      <c r="D88" t="s">
-        <v>86</v>
-      </c>
-      <c r="E88" t="s">
-        <v>86</v>
-      </c>
-      <c r="F88" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+      <c r="B88" s="2"/>
+      <c r="C88" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C89" t="s">
-        <v>86</v>
-      </c>
-      <c r="D89" t="s">
-        <v>86</v>
-      </c>
-      <c r="E89" t="s">
-        <v>86</v>
-      </c>
-      <c r="F89" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+      <c r="B89" s="2"/>
+      <c r="C89" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C90" t="s">
-        <v>86</v>
-      </c>
-      <c r="D90" t="s">
-        <v>86</v>
-      </c>
-      <c r="F90" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+      <c r="B90" s="2"/>
+      <c r="C90" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E90" s="2"/>
+      <c r="F90" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C91" t="s">
+      <c r="B91" s="2"/>
+      <c r="C91" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E91" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F91" t="s">
+      <c r="F91" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C92" t="s">
-        <v>86</v>
-      </c>
-      <c r="E92" t="s">
-        <v>86</v>
-      </c>
-      <c r="F92" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+      <c r="B92" s="2"/>
+      <c r="C92" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C93" t="s">
+      <c r="B93" s="2"/>
+      <c r="C93" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D93" s="5"/>
-      <c r="E93" t="s">
+      <c r="D93" s="2"/>
+      <c r="E93" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F93" t="s">
+      <c r="F93" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C94" t="s">
+      <c r="B94" s="2"/>
+      <c r="C94" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F94" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C95" t="s">
+      <c r="B95" s="2"/>
+      <c r="C95" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D95" t="s">
-        <v>86</v>
-      </c>
-      <c r="F95" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="5" t="s">
+      <c r="D95" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E95" s="2"/>
+      <c r="F95" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C96" s="5"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="5"/>
-      <c r="F96" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C97" t="s">
-        <v>86</v>
-      </c>
-      <c r="D97" t="s">
-        <v>86</v>
-      </c>
-      <c r="F97" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="5" t="s">
+      <c r="B97" s="2"/>
+      <c r="C97" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E97" s="2"/>
+      <c r="F97" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C98" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="5" t="s">
+      <c r="B98" s="2"/>
+      <c r="C98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C99" s="5"/>
-      <c r="D99" s="5"/>
-      <c r="E99" s="5"/>
-      <c r="F99" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="5" t="s">
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C100" s="5"/>
-      <c r="D100" s="5"/>
-      <c r="E100" s="5"/>
-      <c r="F100" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C101" t="s">
-        <v>86</v>
-      </c>
-      <c r="D101" t="s">
-        <v>86</v>
-      </c>
-      <c r="E101" t="s">
-        <v>86</v>
-      </c>
-      <c r="F101" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F102"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="2"/>
+      <c r="F102" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F101" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
@@ -2943,7 +3181,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>